<commit_message>
monitoring_report_v1.5 adding new sheet
</commit_message>
<xml_diff>
--- a/data_import/pending.xlsx
+++ b/data_import/pending.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -596,22 +596,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P-22/074-S00</t>
+          <t>P-22/075-S00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>22-12-2022</t>
+          <t>09-12-2022</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>10-07-2023</t>
+          <t>27-06-2023</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>104001091</t>
+          <t>104001071</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -621,27 +621,27 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Caudal</t>
+          <t>Nivel</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>V-1040010910-0010</t>
+          <t>V-1040010710-0003</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>22-074-PRC-0016</t>
+          <t>22-075-PLN-0001</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>PAINTING PROCEDURE</t>
+          <t>QUALITY CONTROL PLAN 22-075</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Pintura</t>
+          <t>PPI</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -651,45 +651,45 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Com. Mayores</t>
+          <t>Com. Menores</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>17-04-2024</t>
+          <t>24-05-2024</t>
         </is>
       </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
         <is>
-          <t>29-01-2024 Enviado Rev. 0 // 07-02-2024 Rechazado Rev. 1 // 12-04-2024 Enviado Rev. 1 // 17-04-2024 Com. Mayores Rev. 1</t>
+          <t>31-10-2023 Comentado Rev. 2 // 07-11-2023 Enviado Rev. 3 // 21-12-2023 Com. Menores Rev. 3 // 05-01-2024 Enviado Rev. 4 // 07-02-2024 Com. Menores Rev. 5 // 14-02-2024 Enviado Rev. 5 // 24-05-2024 Com. Menores Rev. 5</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P-22/074-S00</t>
+          <t>P-22/075-S00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>22-12-2022</t>
+          <t>09-12-2022</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>10-07-2023</t>
+          <t>27-06-2023</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>104001091</t>
+          <t>104001071</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -699,37 +699,37 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Caudal</t>
+          <t>Nivel</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>V-1040010910-0002</t>
+          <t>V-1040010710-0026</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>22-074-PLG-0005</t>
+          <t>22-075-PRC-0016</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>OVERALL DRAWING WITH WEIGHT FOR FE &amp; FO (ARZANAH)</t>
+          <t>PAINTING PROCEDURE</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Planos</t>
+          <t>Pintura</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Sí</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Com. Menores</t>
+          <t>Rechazado</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -739,35 +739,39 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>22-05-2024</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr"/>
+          <t>06-02-2024</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Se encuentra en estado de HOLD todo el pedido</t>
+        </is>
+      </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>05-01-2024 Enviado Rev. 0 // 22-02-2024 Com. Mayores Rev. 1 // 22-03-2024 Enviado Rev. 1 // 22-05-2024 Com. Menores Rev. 1</t>
+          <t>26-01-2024 Enviado Rev. 0 // 26-01-2024 Rechazado Rev. 1 // 06-02-2024 Com. Mayores Rev. 1 // 06-02-2024 Rechazado Rev. 1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P-22/075-S00</t>
+          <t>P-23/028-S00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>09-12-2022</t>
+          <t>28-02-2023</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>27-06-2023</t>
+          <t>26-10-2023</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>104001071</t>
+          <t>103701061</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -777,27 +781,27 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Nivel</t>
+          <t>Temperatura</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>V-1040010710-0003</t>
+          <t>3998_18-1037010610-00013</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>22-075-PLN-0001</t>
+          <t>23-028-PRC-0009</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>QUALITY CONTROL PLAN 22-075</t>
+          <t>NFXP3 - PRESERVATION AND STORAGE INSTRUCTIONS - THERMOMETERS WITH WELL</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>PPI</t>
+          <t>Instrucciones</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -812,40 +816,44 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>24-05-2024</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr"/>
+          <t>03-07-2024</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>En eGesdoc el doc. Eipsa es: 23-028-DOS-0001</t>
+        </is>
+      </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>31-10-2023 Comentado Rev. 2 // 07-11-2023 Enviado Rev. 3 // 21-12-2023 Com. Menores Rev. 3 // 05-01-2024 Enviado Rev. 4 // 07-02-2024 Com. Menores Rev. 5 // 14-02-2024 Enviado Rev. 5 // 24-05-2024 Com. Menores Rev. 5</t>
+          <t>22-02-2024 Com. Menores Rev. 2 // 26-02-2024 Enviado Rev. 3 // 06-05-2024 Com. Menores Rev. 3 // 06-05-2024 Enviado Rev. 4 // 03-07-2024 Com. Menores Rev. 4</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P-22/075-S00</t>
+          <t>P-23/036-S00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>09-12-2022</t>
+          <t>28-03-2023</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>27-06-2023</t>
+          <t>23-11-2023</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>104001071</t>
+          <t>RFQ 12-99-52-1807 _REV.A</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -855,79 +863,79 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Nivel</t>
+          <t>Caudal</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>V-1040010710-0026</t>
+          <t>8005710911-V-0011</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>22-075-PRC-0016</t>
+          <t>23-036-DOS-0002</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>PAINTING PROCEDURE</t>
+          <t>FINAL QUALITY DOSSIER</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Pintura</t>
+          <t>Dossier</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Sí</t>
+          <t>No</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Rechazado</t>
+          <t>Com. Menores</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>06-02-2024</t>
+          <t>14-06-2024</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Se encuentra en estado de HOLD todo el pedido</t>
+          <t>Este pedido esta terminado. Mientras no reclamen no vamos ha enviar nada. Entra a fecha 14/06/2024 Aceptado con Com.Menores</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>26-01-2024 Enviado Rev. 0 // 26-01-2024 Rechazado Rev. 1</t>
+          <t>24-07-2023 Aprobado Rev. 0 // 14-06-2024 Com. Menores Rev. 0</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P-23/044-S00</t>
+          <t>P-23/048-S00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>26-04-2023</t>
+          <t>12-05-2023</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>22-12-2023</t>
+          <t>07-01-2024</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>103701091</t>
+          <t>104301071</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -937,32 +945,32 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Caudal</t>
+          <t>Nivel</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>3998_18-1037010910-00003</t>
+          <t>5022_20-1043010710-00004</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>23-044-DOS-0001</t>
+          <t>23-048-DOS-0002</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>NFXP3 - WELDING PROCEDURE - ORIFICE PLATES, RESTRICTION ORIFICE &amp; VENTURIS</t>
+          <t>NFXP4 - MANUFACTURING RECORDS BOOK FOR LEVEL GAUGES</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Soldadura</t>
+          <t>Dossier</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Sí</t>
+          <t>No</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -972,330 +980,22 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>05-03-2024</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr"/>
+          <t>30-04-2024</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Vuelve a enviar dev. 20/05/24 sin realizar ningún envío</t>
+        </is>
+      </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>13-11-2023 Enviado Rev. 1 // 18-12-2023 Com. Mayores Rev. 1 // 30-01-2024 Enviado Rev. 2 // 05-03-2024 Com. Menores Rev. 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>P-23/044-S04</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>22-03-2024</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>17-07-2024</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>1037010910-04</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>TÉCNICAS REUNIDAS</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Caudal</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>3998_18-1037010910-00047</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>23-044-S04-PLG-0005-129C-2</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>NFXP3 - CALCULATIONS AND OVERALL DRAWINGS FOR RESTRICTION ORIFICE - RLTO LPB 31 - S04</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Cálculo y plano</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Com. Menores</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>23-05-2024</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>29-04-2024 Enviado Rev. 0 // 23-05-2024 Com. Menores Rev. 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>P-23/048-S00</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>12-05-2023</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>07-01-2024</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>104301071</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>TÉCNICAS REUNIDAS</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Nivel</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>5022_20-1043010710-00004</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>23-048-DOS-0002</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>NFXP4 - MANUFACTURING RECORDS BOOK FOR LEVEL GAUGES</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Dossier</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>Com. Menores</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>30-04-2024</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>Vuelve a enviar dev. 20/05/24 sin realizar ningún envío</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
           <t>25-04-2024 Enviado Rev. 0 // 30-04-2024 Com. Menores Rev. 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>P-23/075-S00</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>01-09-2023</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>07-11-2023</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>7023010412</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>TÉCNICAS REUNIDAS</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Temperatura</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>70230-00-CQY-GLJ-EPS-001</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>23-075-LIS-0017</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>SPARE PARTS LIST FOR 2 YEARS OF OPERATION</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Repuestos</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>Com. Menores</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>20-05-2024</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>16-05-2024 Enviado Rev. 0 // 20-05-2024 Com. Menores Rev. 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>P-23/076-S00</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>01-09-2023</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>07-11-2023</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>7024010412</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>TÉCNICAS REUNIDAS</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Temperatura</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>23-076-LIS-0017</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>SPARE PARTS LIST FOR 2 YEARS OF OPERATION</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Repuestos</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>Com. Menores</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>21-05-2024</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>16-05-2024 Enviado Rev. 0 // 21-05-2024 Com. Menores Rev. 0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add databarrule to sheet 'STATUS GLOBAL'
</commit_message>
<xml_diff>
--- a/data_import/pending.xlsx
+++ b/data_import/pending.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -596,22 +596,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P-22/075-S00</t>
+          <t>P-22/074-S00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>09-12-2022</t>
+          <t>22-12-2022</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>27-06-2023</t>
+          <t>10-07-2023</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>104001071</t>
+          <t>104001091</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -621,27 +621,27 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Nivel</t>
+          <t>Caudal</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>V-1040010710-0003</t>
+          <t>V-1040010910-0002</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>22-075-PLN-0001</t>
+          <t>22-074-PLG-0005</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>QUALITY CONTROL PLAN 22-075</t>
+          <t>OVERALL DRAWING WITH WEIGHT FOR FE &amp; FO (ARZANAH)</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>PPI</t>
+          <t>Planos</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -656,18 +656,18 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>24-05-2024</t>
+          <t>12-07-2024</t>
         </is>
       </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
         <is>
-          <t>31-10-2023 Comentado Rev. 2 // 07-11-2023 Enviado Rev. 3 // 21-12-2023 Com. Menores Rev. 3 // 05-01-2024 Enviado Rev. 4 // 07-02-2024 Com. Menores Rev. 5 // 14-02-2024 Enviado Rev. 5 // 24-05-2024 Com. Menores Rev. 5</t>
+          <t>05-01-2024 Enviado Rev. 0 // 22-02-2024 Com. Mayores Rev. 1 // 22-03-2024 Enviado Rev. 1 // 22-05-2024 Com. Menores Rev. 1 // 29-05-2024 Enviado Rev. 2 // 12-07-2024 Com. Menores Rev. 2</t>
         </is>
       </c>
     </row>
@@ -756,22 +756,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P-23/028-S00</t>
+          <t>P-22/075-S00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>28-02-2023</t>
+          <t>09-12-2022</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>26-10-2023</t>
+          <t>27-06-2023</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>103701061</t>
+          <t>104001071</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -781,32 +781,32 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Temperatura</t>
+          <t>Nivel</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>3998_18-1037010610-00013</t>
+          <t>V-1040010710-0003</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>23-028-PRC-0009</t>
+          <t>22-075-PLN-0001</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>NFXP3 - PRESERVATION AND STORAGE INSTRUCTIONS - THERMOMETERS WITH WELL</t>
+          <t>QUALITY CONTROL PLAN 22-075</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Instrucciones</t>
+          <t>PPI</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Sí</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -816,44 +816,40 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>03-07-2024</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>En eGesdoc el doc. Eipsa es: 23-028-DOS-0001</t>
-        </is>
-      </c>
+          <t>24-05-2024</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr">
         <is>
-          <t>22-02-2024 Com. Menores Rev. 2 // 26-02-2024 Enviado Rev. 3 // 06-05-2024 Com. Menores Rev. 3 // 06-05-2024 Enviado Rev. 4 // 03-07-2024 Com. Menores Rev. 4</t>
+          <t>31-10-2023 Comentado Rev. 2 // 07-11-2023 Enviado Rev. 3 // 21-12-2023 Com. Menores Rev. 3 // 05-01-2024 Enviado Rev. 4 // 07-02-2024 Com. Menores Rev. 5 // 14-02-2024 Enviado Rev. 5 // 24-05-2024 Com. Menores Rev. 5</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P-23/036-S00</t>
+          <t>P-23/028-S00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>28-03-2023</t>
+          <t>28-02-2023</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>23-11-2023</t>
+          <t>26-10-2023</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>RFQ 12-99-52-1807 _REV.A</t>
+          <t>103701061</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -863,27 +859,27 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Caudal</t>
+          <t>Temperatura</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>8005710911-V-0011</t>
+          <t>3998_18-1037010610-00014</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>23-036-DOS-0002</t>
+          <t>23-028-PRC-0012</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>FINAL QUALITY DOSSIER</t>
+          <t>PACKING &amp; TRANSPORTATION PROCEDURE</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Dossier</t>
+          <t>Packing</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -898,44 +894,40 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>14-06-2024</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>Este pedido esta terminado. Mientras no reclamen no vamos ha enviar nada. Entra a fecha 14/06/2024 Aceptado con Com.Menores</t>
-        </is>
-      </c>
+          <t>17-07-2024</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr">
         <is>
-          <t>24-07-2023 Aprobado Rev. 0 // 14-06-2024 Com. Menores Rev. 0</t>
+          <t>11-12-2023 Com. Menores Rev. 0 // 15-02-2024 Enviado Rev. 0 // 11-06-2024 Com. Menores Rev. 0 // 11-06-2024 Enviado Rev. 1 // 17-07-2024 Com. Menores Rev. 1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P-23/048-S00</t>
+          <t>P-23/036-S00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>12-05-2023</t>
+          <t>28-03-2023</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>07-01-2024</t>
+          <t>23-11-2023</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>104301071</t>
+          <t>RFQ 12-99-52-1807 _REV.A</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -945,22 +937,22 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Nivel</t>
+          <t>Caudal</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>5022_20-1043010710-00004</t>
+          <t>8005710911-V-0011</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>23-048-DOS-0002</t>
+          <t>23-036-DOS-0002</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>NFXP4 - MANUFACTURING RECORDS BOOK FOR LEVEL GAUGES</t>
+          <t>FINAL QUALITY DOSSIER</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -985,17 +977,95 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>30-04-2024</t>
+          <t>14-06-2024</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Vuelve a enviar dev. 20/05/24 sin realizar ningún envío</t>
+          <t>Este pedido esta terminado. Mientras no reclamen no vamos ha enviar nada. Entra a fecha 14/06/2024 Aceptado con Com.Menores</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>25-04-2024 Enviado Rev. 0 // 30-04-2024 Com. Menores Rev. 0</t>
+          <t>24-07-2023 Aprobado Rev. 0 // 14-06-2024 Com. Menores Rev. 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>P-23/044-S05</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>31-05-2024</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>22-07-2024</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1037010910-05</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>TÉCNICAS REUNIDAS</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Caudal</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>3998_18-1037010910-00051</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>23-044-S05-PLG-0005-B18</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>NFXP3 - BARZAN ISBL - CALCULATIONS AND OVERALL DRAWINGS FOR RESTRICTION ORIFICE</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Cálculo y plano</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Com. Menores</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>17-07-2024</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>24-05-2024 Enviado Rev. 0 // 25-06-2024 Com. Menores Rev. 0 // 26-06-2024 Enviado Rev. 1 // 17-07-2024 Com. Menores Rev. 1</t>
         </is>
       </c>
     </row>

</xml_diff>